<commit_message>
tire à l'eau coulé manquant
</commit_message>
<xml_diff>
--- a/doc/Documentation de projet/Résultats de test.xlsx
+++ b/doc/Documentation de projet/Résultats de test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="11415"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="11415"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>14.03.2019 Mounir Fiaux windows 10</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>quitter le jeu</t>
+  </si>
+  <si>
+    <t>afficher touché couler et à l'eau</t>
+  </si>
+  <si>
+    <t>créer les grilles aléatoirement</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -293,16 +299,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
       <border>
@@ -321,12 +332,10 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
       <border>
@@ -628,7 +637,7 @@
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +671,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="L1" s="3"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -683,15 +692,19 @@
       <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -712,15 +725,19 @@
       <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
@@ -741,15 +758,19 @@
       <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="L4" s="11"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
@@ -770,15 +791,19 @@
       <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
@@ -796,14 +821,16 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
@@ -828,7 +855,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+      <c r="L7" s="11"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
@@ -839,16 +866,12 @@
       <c r="T7" s="10"/>
       <c r="U7" s="11"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>6</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -857,7 +880,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
@@ -868,16 +891,12 @@
       <c r="T8" s="10"/>
       <c r="U8" s="11"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>6</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -886,7 +905,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
@@ -898,18 +917,28 @@
       <c r="U9" s="11"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
@@ -921,18 +950,28 @@
       <c r="U10" s="11"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
@@ -944,27 +983,27 @@
       <c r="U11" s="11"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="11"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="18"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
@@ -978,7 +1017,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1001,7 +1040,7 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -1024,7 +1063,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -1035,19 +1074,19 @@
       <c r="T15" s="10"/>
       <c r="U15" s="11"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
+    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="14"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -1427,12 +1466,12 @@
       <c r="U32" s="14"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U32">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="OK">
+  <conditionalFormatting sqref="B13:U32 B2:U11">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="KO">
+      <formula>NOT(ISERROR(SEARCH("KO",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="KO">
-      <formula>NOT(ISERROR(SEARCH("KO",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>